<commit_message>
added the creation of the xlsx file
</commit_message>
<xml_diff>
--- a/my_function/output_file.xlsx
+++ b/my_function/output_file.xlsx
@@ -124,10 +124,10 @@
     <t xml:space="preserve"> RDS DB Instance is currently not in AVAILABLE state. Current state: stopped."</t>
   </si>
   <si>
-    <t>2023-12-10T21:00:00Z</t>
-  </si>
-  <si>
-    <t>2023-12-10T22:00:00Z</t>
+    <t>2023-12-11T21:00:00Z</t>
+  </si>
+  <si>
+    <t>2023-12-11T22:00:00Z</t>
   </si>
   <si>
     <t>"2f9ee359-0265-3ca4-ab2c-289cd54d6705"</t>

</xml_diff>